<commit_message>
update table and add epen
</commit_message>
<xml_diff>
--- a/plot_traj/robocane_exp/hst.xlsx
+++ b/plot_traj/robocane_exp/hst.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="149">
   <si>
     <t>Subject</t>
   </si>
@@ -470,6 +470,9 @@
   </si>
   <si>
     <t>(31.25, 9.38,0.02)</t>
+  </si>
+  <si>
+    <t>elevator (35.5,1.1,0)</t>
   </si>
 </sst>
 </file>
@@ -998,7 +1001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
@@ -2373,7 +2376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -3611,10 +3614,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:L18"/>
+  <dimension ref="D3:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3800,6 +3803,11 @@
         <v>119</v>
       </c>
     </row>
+    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>148</v>
+      </c>
+    </row>
     <row r="13" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>72</v>
@@ -3877,7 +3885,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>103</v>
       </c>
@@ -3903,7 +3911,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>111</v>
       </c>
@@ -3929,9 +3937,249 @@
         <v>145</v>
       </c>
     </row>
+    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D22" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+    </row>
+    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" t="s">
+        <v>75</v>
+      </c>
+      <c r="I23" t="s">
+        <v>76</v>
+      </c>
+      <c r="J23" t="s">
+        <v>77</v>
+      </c>
+      <c r="K23" t="s">
+        <v>78</v>
+      </c>
+      <c r="L23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24">
+        <v>1.59</v>
+      </c>
+      <c r="F24">
+        <v>0.54</v>
+      </c>
+      <c r="G24">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="H24">
+        <v>0.74</v>
+      </c>
+      <c r="I24">
+        <v>0.97</v>
+      </c>
+      <c r="J24">
+        <v>0.59</v>
+      </c>
+      <c r="K24">
+        <v>1.51</v>
+      </c>
+      <c r="L24">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="H25">
+        <v>1.44</v>
+      </c>
+      <c r="I25">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="K25">
+        <v>2.56</v>
+      </c>
+      <c r="L25">
+        <v>4.38</v>
+      </c>
+    </row>
+    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26">
+        <v>1.48</v>
+      </c>
+      <c r="G26">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="I26">
+        <v>2.36</v>
+      </c>
+      <c r="J26">
+        <v>1.89</v>
+      </c>
+      <c r="K26">
+        <v>3.33</v>
+      </c>
+      <c r="L26">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>111</v>
+      </c>
+      <c r="E28">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="F28">
+        <v>0.62</v>
+      </c>
+      <c r="G28">
+        <v>0.67</v>
+      </c>
+      <c r="H28">
+        <v>1.94</v>
+      </c>
+      <c r="I28">
+        <v>0.64</v>
+      </c>
+      <c r="J28">
+        <v>0.65</v>
+      </c>
+      <c r="K28">
+        <v>1.89</v>
+      </c>
+      <c r="L28">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="32" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" t="s">
+        <v>74</v>
+      </c>
+      <c r="H33" t="s">
+        <v>75</v>
+      </c>
+      <c r="I33" t="s">
+        <v>76</v>
+      </c>
+      <c r="J33" t="s">
+        <v>77</v>
+      </c>
+      <c r="K33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>80</v>
+      </c>
+      <c r="F34">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G34">
+        <v>0.99</v>
+      </c>
+      <c r="H34">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="I34">
+        <v>7.37</v>
+      </c>
+      <c r="J34">
+        <v>6.01</v>
+      </c>
+      <c r="K34">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>89</v>
+      </c>
+      <c r="H35">
+        <v>9.07</v>
+      </c>
+      <c r="I35">
+        <v>5.53</v>
+      </c>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>96</v>
+      </c>
+      <c r="J36">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="K36">
+        <v>13.75</v>
+      </c>
+    </row>
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>111</v>
+      </c>
+      <c r="F38">
+        <v>1.04</v>
+      </c>
+      <c r="G38">
+        <v>2.29</v>
+      </c>
+      <c r="H38">
+        <v>1.55</v>
+      </c>
+      <c r="I38">
+        <v>1.23</v>
+      </c>
+      <c r="J38">
+        <v>0.7</v>
+      </c>
+      <c r="K38">
+        <v>2.5499999999999998</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D3:L3"/>
+    <mergeCell ref="D22:L22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update new forward data
</commit_message>
<xml_diff>
--- a/plot_traj/robocane_exp/hst.xlsx
+++ b/plot_traj/robocane_exp/hst.xlsx
@@ -1,32 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hzhang8\Desktop\work\code\slam_matlab\plot_traj\robocane_exp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuyin\Desktop\work\code\github\slam_matlab\slam_matlab\plot_traj\robocane_exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73D3EDC-FF0B-4A97-A806-238756A6A5AB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16635" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="24000" windowHeight="8940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Without" sheetId="2" r:id="rId1"/>
     <sheet name="With" sheetId="4" r:id="rId2"/>
     <sheet name="traj" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="261">
   <si>
     <t>Subject</t>
   </si>
@@ -473,16 +482,352 @@
   </si>
   <si>
     <t>elevator (35.5,1.1,0)</t>
+  </si>
+  <si>
+    <t>Straight Slow (0, 20, 0)</t>
+  </si>
+  <si>
+    <t>(0.28,18.95,-0.02)</t>
+  </si>
+  <si>
+    <t>(0.45,19.13,0.28)</t>
+  </si>
+  <si>
+    <t>(0.73,18.25,0.54)</t>
+  </si>
+  <si>
+    <t>(0.41, 18.14,0.09)</t>
+  </si>
+  <si>
+    <t>(1.16,19.52,-0.1)</t>
+  </si>
+  <si>
+    <t>Straight Fast</t>
+  </si>
+  <si>
+    <t>(0.4,17.96,0.28)</t>
+  </si>
+  <si>
+    <t>(0.43,19.69,0.63)</t>
+  </si>
+  <si>
+    <t>(-0.1,19.31,0.18)</t>
+  </si>
+  <si>
+    <t>(0.35, 20.17,0.21)</t>
+  </si>
+  <si>
+    <t>(0.73,19.59,-0.0)</t>
+  </si>
+  <si>
+    <t>Swing Slow</t>
+  </si>
+  <si>
+    <t>Swing Fast</t>
+  </si>
+  <si>
+    <t>(1.02,19.18,0.23)</t>
+  </si>
+  <si>
+    <t>(0.77,20.07,0.26)</t>
+  </si>
+  <si>
+    <t>(-0.42,20.15,0.13)</t>
+  </si>
+  <si>
+    <t>(0.44,19.42,0.43)</t>
+  </si>
+  <si>
+    <t>(0.58, 21.66, 0.50)</t>
+  </si>
+  <si>
+    <t>(1.83, 20.78, 0.23)</t>
+  </si>
+  <si>
+    <t>(0.72, 20.65, 0.44)</t>
+  </si>
+  <si>
+    <t>(1.46,19.54,0.27)</t>
+  </si>
+  <si>
+    <t>(0.51,20.76,0.08)</t>
+  </si>
+  <si>
+    <t>(1.03,21.32,0.26)</t>
+  </si>
+  <si>
+    <t>(-0.56,20.23,0.22)</t>
+  </si>
+  <si>
+    <t>(-4.67, 26.32,-0.38)</t>
+  </si>
+  <si>
+    <t>(-1.8, 25.67, -0.78)</t>
+  </si>
+  <si>
+    <t>(-2.6, 23.0,-1.1)</t>
+  </si>
+  <si>
+    <t>(-0.68, 22.72, -0.53)</t>
+  </si>
+  <si>
+    <t>(-2.75, 24.98,-0.63)</t>
+  </si>
+  <si>
+    <t>(-1.39, 19.37,0.3)</t>
+  </si>
+  <si>
+    <t>(-2.48, 20.25, -0.11)</t>
+  </si>
+  <si>
+    <t>(-2.04, 21.53,-0.11)</t>
+  </si>
+  <si>
+    <t>(-1.97, 22.00, -0.32)</t>
+  </si>
+  <si>
+    <t>(-1.31, 21.35,-0.08)</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>(-3.43, 15.2, -1.41)</t>
+  </si>
+  <si>
+    <t>(-2.18, 15.54, -0.74)</t>
+  </si>
+  <si>
+    <t>(-1.97, 15.43,-0.31)</t>
+  </si>
+  <si>
+    <t>(-0.75, 14.07, -0.22)</t>
+  </si>
+  <si>
+    <t>(-0.33,15.96,-1.15)</t>
+  </si>
+  <si>
+    <t>(-3.61, 14.99,-0.76)</t>
+  </si>
+  <si>
+    <t>(-1.06,14.49,-0.72)</t>
+  </si>
+  <si>
+    <t>(-1.49, 14.2,-0.71)</t>
+  </si>
+  <si>
+    <t>(-1.88,14.84,-0.87)</t>
+  </si>
+  <si>
+    <t>(-1.36, 15.4,-0.47)</t>
+  </si>
+  <si>
+    <t>(-0.4, 18.79,0.26)</t>
+  </si>
+  <si>
+    <t>(0.30, 19.13,0.27)</t>
+  </si>
+  <si>
+    <t>(-0.46, 18.53,-0.04)</t>
+  </si>
+  <si>
+    <t>(-0.05, 18.08,0.07)</t>
+  </si>
+  <si>
+    <t>(-1.47, 18.69,0.08)</t>
+  </si>
+  <si>
+    <t>(-0.69, 17.8,0.09)</t>
+  </si>
+  <si>
+    <t>(-0.6, 18.41,-0.02)</t>
+  </si>
+  <si>
+    <t>(0.018, 18.63,-0.21)</t>
+  </si>
+  <si>
+    <t>(-0.8, 18.46,-0.023)</t>
+  </si>
+  <si>
+    <t>(0.04, 18.77,-0.022)</t>
+  </si>
+  <si>
+    <t>0.93, 19.34,-0.03)</t>
+  </si>
+  <si>
+    <t>(0.56, 18.92,-0.02)</t>
+  </si>
+  <si>
+    <t>(-0.06, 19.24,0.1)</t>
+  </si>
+  <si>
+    <t>(-0.51, 18.46,0.13)</t>
+  </si>
+  <si>
+    <t>(-2.23, 19.02,-0.05)</t>
+  </si>
+  <si>
+    <t>(-2.49, 19.0, 0.25)</t>
+  </si>
+  <si>
+    <t>(0.33,19.48,-0.24)</t>
+  </si>
+  <si>
+    <t>(-1.11, 17.95,0.15)</t>
+  </si>
+  <si>
+    <t>(1.18, 19.32,-0.02)</t>
+  </si>
+  <si>
+    <t>(-1.89, 19.31,-0.036)</t>
+  </si>
+  <si>
+    <t>(-1.77, 18.35,-0.1)</t>
+  </si>
+  <si>
+    <t>(-0.61, 18.73,-0.05)</t>
+  </si>
+  <si>
+    <t>(-1.2, 19.43,0.21)</t>
+  </si>
+  <si>
+    <t>(-0.07,19.25,-0.46)</t>
+  </si>
+  <si>
+    <t>(0.08,18.68,0.94)</t>
+  </si>
+  <si>
+    <t>(-0.13, 19.18,0.17)</t>
+  </si>
+  <si>
+    <t>(-0.16,19.0,0.09)</t>
+  </si>
+  <si>
+    <t>(0.4,18.44,0.42)</t>
+  </si>
+  <si>
+    <t>(-0.2,20.08,0.77)</t>
+  </si>
+  <si>
+    <t>(-0.8,21.4,-0.29)</t>
+  </si>
+  <si>
+    <t>(-0.42, 18.4,-0.09)</t>
+  </si>
+  <si>
+    <t>(-0.73,20.35,0.89)</t>
+  </si>
+  <si>
+    <t>(-0.74,19.31,0.42)</t>
+  </si>
+  <si>
+    <t>(-0.51,20.12,0.23)</t>
+  </si>
+  <si>
+    <t>(1.65,20.19,-0.04)</t>
+  </si>
+  <si>
+    <t>(0.01,18.87,0.82)</t>
+  </si>
+  <si>
+    <t>(0.82, 19.26, 0.41)</t>
+  </si>
+  <si>
+    <t>(0.67,18.79,0.43)</t>
+  </si>
+  <si>
+    <t>(0.09,19.61,0.11)</t>
+  </si>
+  <si>
+    <t>(0.13, 18.96,0.38)</t>
+  </si>
+  <si>
+    <t>(-0.16, 19.96,-0.01)</t>
+  </si>
+  <si>
+    <t>(-1.7, 19.8,-0.03)</t>
+  </si>
+  <si>
+    <t>(-0.41, 19.92,-0.00)</t>
+  </si>
+  <si>
+    <t>(-1.6, 19.69,0.00)</t>
+  </si>
+  <si>
+    <t>(-1.78, 19.84,-0.01)</t>
+  </si>
+  <si>
+    <t>(-2.22, 19.5,-0.01)</t>
+  </si>
+  <si>
+    <t>(-1.07, 19.1, 0.00)</t>
+  </si>
+  <si>
+    <t>(-1.6, 19.29,-0.01)</t>
+  </si>
+  <si>
+    <t>(-0.38, 19.57,-0.01)</t>
+  </si>
+  <si>
+    <t>(-1.16, 19.43,0.)</t>
+  </si>
+  <si>
+    <t>(-1.42, 19.05,-0.00)</t>
+  </si>
+  <si>
+    <t>(-1.21, 18.86,-0.01)</t>
+  </si>
+  <si>
+    <t>(-1.11, 19.26,0.00)</t>
+  </si>
+  <si>
+    <t>(-0.89, 19.39,0.01)</t>
+  </si>
+  <si>
+    <t>(-1.31, 18.88,0.00)</t>
+  </si>
+  <si>
+    <t>(-3.03, 19.25,0.03)</t>
+  </si>
+  <si>
+    <t>(2.22, 18.64,0.00)</t>
+  </si>
+  <si>
+    <t>(-1.44, 19.29,-0.0)</t>
+  </si>
+  <si>
+    <t>(1.17, 18.77,0.01)</t>
+  </si>
+  <si>
+    <t>(-1.89,25.26,0.07)</t>
+  </si>
+  <si>
+    <t>(-2.1,25.15,-0.28)</t>
+  </si>
+  <si>
+    <t>(-1.65,18.12,0.11)</t>
+  </si>
+  <si>
+    <t>(-1.79,22.11,1.23)</t>
+  </si>
+  <si>
+    <t>(-1.35,15.5,-0.56)</t>
+  </si>
+  <si>
+    <t>(0.47, 15.45, 0.11)</t>
+  </si>
+  <si>
+    <t>(-0.81,15.54,-0.66)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -505,8 +850,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -535,6 +894,16 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -634,10 +1003,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -685,9 +1056,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="好" xfId="1" builtinId="26"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="适中" xfId="2" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -998,7 +1373,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
@@ -2373,7 +2748,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3613,11 +3988,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="D3:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4183,4 +4558,795 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{202F8189-52C6-4F0C-88CE-8CCBC1727F3F}">
+  <dimension ref="C4:J38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.875" customWidth="1"/>
+    <col min="5" max="5" width="20.125" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="8" width="17.375" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="10" max="10" width="15.25" customWidth="1"/>
+    <col min="11" max="11" width="25.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="G6" t="s">
+        <v>198</v>
+      </c>
+      <c r="H6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="32"/>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="G8" t="s">
+        <v>177</v>
+      </c>
+      <c r="H8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="G9" t="s">
+        <v>153</v>
+      </c>
+      <c r="H9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" t="s">
+        <v>200</v>
+      </c>
+      <c r="E16" t="s">
+        <v>202</v>
+      </c>
+      <c r="F16" t="s">
+        <v>201</v>
+      </c>
+      <c r="G16" t="s">
+        <v>203</v>
+      </c>
+      <c r="H16" s="31" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="31"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" t="s">
+        <v>179</v>
+      </c>
+      <c r="E18" t="s">
+        <v>180</v>
+      </c>
+      <c r="F18" t="s">
+        <v>181</v>
+      </c>
+      <c r="G18" t="s">
+        <v>182</v>
+      </c>
+      <c r="H18" s="31" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" t="s">
+        <v>156</v>
+      </c>
+      <c r="E19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F19" t="s">
+        <v>158</v>
+      </c>
+      <c r="G19" t="s">
+        <v>159</v>
+      </c>
+      <c r="H19" s="31" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D22" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" t="s">
+        <v>75</v>
+      </c>
+      <c r="H23" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" t="s">
+        <v>77</v>
+      </c>
+      <c r="J23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" t="s">
+        <v>205</v>
+      </c>
+      <c r="E24" t="s">
+        <v>206</v>
+      </c>
+      <c r="F24" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="G24" t="s">
+        <v>208</v>
+      </c>
+      <c r="H24" t="s">
+        <v>209</v>
+      </c>
+      <c r="I24" t="s">
+        <v>210</v>
+      </c>
+      <c r="J24" s="31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25" s="31"/>
+      <c r="J25" s="31"/>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" t="s">
+        <v>184</v>
+      </c>
+      <c r="E26" t="s">
+        <v>185</v>
+      </c>
+      <c r="F26" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="G26" t="s">
+        <v>186</v>
+      </c>
+      <c r="H26" t="s">
+        <v>187</v>
+      </c>
+      <c r="I26" t="s">
+        <v>188</v>
+      </c>
+      <c r="J26" s="31" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" t="s">
+        <v>163</v>
+      </c>
+      <c r="E27" t="s">
+        <v>164</v>
+      </c>
+      <c r="F27" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="G27" t="s">
+        <v>166</v>
+      </c>
+      <c r="H27" t="s">
+        <v>167</v>
+      </c>
+      <c r="I27" t="s">
+        <v>168</v>
+      </c>
+      <c r="J27" s="31" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D33" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" t="s">
+        <v>74</v>
+      </c>
+      <c r="G34" t="s">
+        <v>75</v>
+      </c>
+      <c r="H34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" t="s">
+        <v>212</v>
+      </c>
+      <c r="E35" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="F35" t="s">
+        <v>214</v>
+      </c>
+      <c r="G35" t="s">
+        <v>215</v>
+      </c>
+      <c r="H35" s="31" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="31"/>
+      <c r="H36" s="31"/>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" t="s">
+        <v>190</v>
+      </c>
+      <c r="E37" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="F37" t="s">
+        <v>192</v>
+      </c>
+      <c r="G37" t="s">
+        <v>193</v>
+      </c>
+      <c r="H37" s="31" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" t="s">
+        <v>170</v>
+      </c>
+      <c r="E38" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="F38" t="s">
+        <v>172</v>
+      </c>
+      <c r="G38" t="s">
+        <v>159</v>
+      </c>
+      <c r="H38" s="31" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="D33:H33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08947BF0-9736-4768-AFB9-DD16CCE2EEA5}">
+  <dimension ref="D4:I38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13.75" customWidth="1"/>
+    <col min="5" max="5" width="16.875" customWidth="1"/>
+    <col min="6" max="6" width="19.25" customWidth="1"/>
+    <col min="7" max="7" width="17.75" customWidth="1"/>
+    <col min="8" max="8" width="22.125" customWidth="1"/>
+    <col min="9" max="9" width="20.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E4" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+    </row>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="F6" t="s">
+        <v>236</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="H6" t="s">
+        <v>238</v>
+      </c>
+      <c r="I6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="31"/>
+      <c r="G7" s="31"/>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="F9" t="s">
+        <v>218</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="H9" t="s">
+        <v>220</v>
+      </c>
+      <c r="I9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E14" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" t="s">
+        <v>75</v>
+      </c>
+      <c r="I15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
+        <v>240</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>241</v>
+      </c>
+      <c r="G16" t="s">
+        <v>242</v>
+      </c>
+      <c r="H16" t="s">
+        <v>243</v>
+      </c>
+      <c r="I16" s="31" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" s="31"/>
+      <c r="I17" s="31"/>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="I18" s="31" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" t="s">
+        <v>222</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="G19" t="s">
+        <v>224</v>
+      </c>
+      <c r="H19" t="s">
+        <v>225</v>
+      </c>
+      <c r="I19" s="31" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E22" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" t="s">
+        <v>75</v>
+      </c>
+      <c r="I23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="F24" t="s">
+        <v>246</v>
+      </c>
+      <c r="G24" t="s">
+        <v>249</v>
+      </c>
+      <c r="H24" s="31" t="s">
+        <v>247</v>
+      </c>
+      <c r="I24" s="31" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+    </row>
+    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="31" t="s">
+        <v>258</v>
+      </c>
+      <c r="H26" s="31" t="s">
+        <v>259</v>
+      </c>
+      <c r="I26" s="31" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="F27" t="s">
+        <v>228</v>
+      </c>
+      <c r="G27" t="s">
+        <v>229</v>
+      </c>
+      <c r="H27" s="31" t="s">
+        <v>230</v>
+      </c>
+      <c r="I27" s="31" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E33" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+    </row>
+    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" t="s">
+        <v>73</v>
+      </c>
+      <c r="G34" t="s">
+        <v>74</v>
+      </c>
+      <c r="H34" t="s">
+        <v>75</v>
+      </c>
+      <c r="I34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" t="s">
+        <v>250</v>
+      </c>
+      <c r="F35" t="s">
+        <v>251</v>
+      </c>
+      <c r="G35" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="H35" t="s">
+        <v>253</v>
+      </c>
+      <c r="I35" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>89</v>
+      </c>
+      <c r="G36" s="32"/>
+    </row>
+    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>96</v>
+      </c>
+      <c r="G37" s="32" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>111</v>
+      </c>
+      <c r="E38" t="s">
+        <v>232</v>
+      </c>
+      <c r="F38" t="s">
+        <v>60</v>
+      </c>
+      <c r="G38" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="H38" t="s">
+        <v>234</v>
+      </c>
+      <c r="I38" t="s">
+        <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E33:I33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>